<commit_message>
used a if loop to be able to use the file as well
</commit_message>
<xml_diff>
--- a/Comp/encoded_elongation_file.xlsx
+++ b/Comp/encoded_elongation_file.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
used KNN to find mech prop and added strong/medium/fragile label to all of the data
</commit_message>
<xml_diff>
--- a/Comp/encoded_elongation_file.xlsx
+++ b/Comp/encoded_elongation_file.xlsx
@@ -695,7 +695,7 @@
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       <c r="Q63" t="inlineStr"/>
       <c r="R63" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -5275,7 +5275,7 @@
       <c r="Q81" t="inlineStr"/>
       <c r="R81" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -5513,7 +5513,7 @@
       <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       <c r="Q96" t="inlineStr"/>
       <c r="R96" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -6941,7 +6941,7 @@
       <c r="Q109" t="inlineStr"/>
       <c r="R109" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -7237,7 +7237,7 @@
       <c r="Q114" t="inlineStr"/>
       <c r="R114" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -7295,7 +7295,7 @@
       <c r="Q115" t="inlineStr"/>
       <c r="R115" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -15005,7 +15005,7 @@
       <c r="Q244" t="inlineStr"/>
       <c r="R244" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -17865,7 +17865,7 @@
       <c r="Q292" t="inlineStr"/>
       <c r="R292" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>

</xml_diff>